<commit_message>
Added something language in projects.
</commit_message>
<xml_diff>
--- a/ExcelFolder/Config.xlsx
+++ b/ExcelFolder/Config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="115">
   <si>
     <t>cache
 export</t>
@@ -158,6 +158,18 @@
     <t>路径配置，语言切换用英文逗号 ”,“ 切割，请勿使用</t>
   </si>
   <si>
+    <t>UnderProjectPath</t>
+  </si>
+  <si>
+    <t>Under The Project Path,在项目路径下</t>
+  </si>
+  <si>
+    <t>NonProjectPath</t>
+  </si>
+  <si>
+    <t>Non-Project Path,非项目路径下</t>
+  </si>
+  <si>
     <t>FrameworkPath</t>
   </si>
   <si>
@@ -182,6 +194,18 @@
     <t>Atlas Save Path:,图集保存路径：</t>
   </si>
   <si>
+    <t>DefaultUIPrefabSavePath</t>
+  </si>
+  <si>
+    <t>Default UI Prefab Save Path: ,默认UI预制件的保存路径：</t>
+  </si>
+  <si>
+    <t>DefaultUICodeSavePath</t>
+  </si>
+  <si>
+    <t>Default Script Save Path: ,默认UI代码保存路径：</t>
+  </si>
+  <si>
     <t>AnimatorExtractPath</t>
   </si>
   <si>
@@ -222,18 +246,6 @@
   </si>
   <si>
     <t>Set Rule Prefixes,组件规则设置</t>
-  </si>
-  <si>
-    <t>DefaultScriptSavePath</t>
-  </si>
-  <si>
-    <t>Default Script Save Path: ,默认组件代码保存路径：</t>
-  </si>
-  <si>
-    <t>DefaultPrefabSavePath</t>
-  </si>
-  <si>
-    <t>Default UI Prefab Save Path: ,默认UI预制件的保存路径：</t>
   </si>
   <si>
     <t>CreatedUIPrefabSavePath</t>
@@ -1391,12 +1403,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1702,23 +1714,37 @@
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" s="3" customFormat="1" spans="1:10">
       <c r="A23" s="12"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" s="3" customFormat="1" spans="1:10">
       <c r="A24" s="12"/>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="19" t="s">
         <v>50</v>
       </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="12"/>
@@ -1747,23 +1773,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:10">
-      <c r="A28" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="15" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="12"/>
@@ -1792,14 +1809,23 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13" t="s">
+    <row r="32" s="2" customFormat="1" spans="1:10">
+      <c r="A32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="16" t="s">
         <v>66</v>
       </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="12"/>
@@ -1873,23 +1899,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" s="2" customFormat="1" spans="1:10">
-      <c r="A41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="15" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="12"/>
@@ -1900,14 +1917,23 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13" t="s">
+    <row r="43" s="2" customFormat="1" spans="1:10">
+      <c r="A43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="16" t="s">
         <v>88</v>
       </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="12"/>
@@ -2006,6 +2032,24 @@
       </c>
       <c r="C54" s="6" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="12"/>
+      <c r="B56" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>